<commit_message>
excell is added to project
</commit_message>
<xml_diff>
--- a/assets/tables/countryTable.xlsx
+++ b/assets/tables/countryTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="948">
   <si>
     <t>country_id</t>
   </si>
@@ -607,6 +607,9 @@
     <t>Cote D'Ivoire</t>
   </si>
   <si>
+    <t>Fildişi Sahili</t>
+  </si>
+  <si>
     <t>CI</t>
   </si>
   <si>
@@ -1573,7 +1576,7 @@
     <t>Micronesia, Federated States of</t>
   </si>
   <si>
-    <t>Mikronezya, federasyonlu durumlar</t>
+    <t>Mikronezya</t>
   </si>
   <si>
     <t>FM</t>
@@ -1903,9 +1906,6 @@
     <t>Pitcairn</t>
   </si>
   <si>
-    <t>Çukur</t>
-  </si>
-  <si>
     <t>PN</t>
   </si>
   <si>
@@ -1963,9 +1963,6 @@
     <t>Reunion</t>
   </si>
   <si>
-    <t>Yeniden birleşme</t>
-  </si>
-  <si>
     <t>RE</t>
   </si>
   <si>
@@ -2369,9 +2366,6 @@
   </si>
   <si>
     <t>Togo</t>
-  </si>
-  <si>
-    <t>Gitmek</t>
   </si>
   <si>
     <t>TG</t>
@@ -2871,7 +2865,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2883,6 +2877,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2924,8 +2924,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -3244,11 +3244,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="41.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="45.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -4143,13 +4143,13 @@
         <v>196</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="12.75">
@@ -4157,16 +4157,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="12.75">
@@ -4174,16 +4174,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="12.75">
@@ -4191,16 +4191,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="12.75">
@@ -4208,16 +4208,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="12.75">
@@ -4225,16 +4225,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="12.75">
@@ -4242,16 +4242,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="12.75">
@@ -4259,16 +4259,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="12.75">
@@ -4276,16 +4276,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="12.75">
@@ -4293,16 +4293,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="12.75">
@@ -4310,16 +4310,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="12.75">
@@ -4327,16 +4327,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="12.75">
@@ -4344,16 +4344,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="12.75">
@@ -4361,16 +4361,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="12.75">
@@ -4378,16 +4378,16 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="12.75">
@@ -4395,16 +4395,16 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="12.75">
@@ -4412,16 +4412,16 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="12.75">
@@ -4429,16 +4429,16 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="12.75">
@@ -4446,16 +4446,16 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="12.75">
@@ -4463,16 +4463,16 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="12.75">
@@ -4480,16 +4480,16 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="12.75">
@@ -4497,16 +4497,16 @@
         <v>74</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="12.75">
@@ -4514,16 +4514,16 @@
         <v>75</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="12.75">
@@ -4531,16 +4531,16 @@
         <v>76</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="12.75">
@@ -4548,16 +4548,16 @@
         <v>77</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="12.75">
@@ -4565,16 +4565,16 @@
         <v>78</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="12.75">
@@ -4582,16 +4582,16 @@
         <v>79</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="12.75">
@@ -4599,16 +4599,16 @@
         <v>80</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="12.75">
@@ -4616,16 +4616,16 @@
         <v>81</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="12.75">
@@ -4633,16 +4633,16 @@
         <v>82</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="12.75">
@@ -4650,16 +4650,16 @@
         <v>83</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="12.75">
@@ -4667,16 +4667,16 @@
         <v>84</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="12.75">
@@ -4684,16 +4684,16 @@
         <v>85</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="12.75">
@@ -4701,16 +4701,16 @@
         <v>86</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="12.75">
@@ -4718,16 +4718,16 @@
         <v>87</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="12.75">
@@ -4735,16 +4735,16 @@
         <v>88</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="12.75">
@@ -4752,16 +4752,16 @@
         <v>89</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="12.75">
@@ -4769,16 +4769,16 @@
         <v>90</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="12.75">
@@ -4786,16 +4786,16 @@
         <v>91</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="12.75">
@@ -4803,16 +4803,16 @@
         <v>92</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="12.75">
@@ -4820,16 +4820,16 @@
         <v>93</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="12.75">
@@ -4837,16 +4837,16 @@
         <v>94</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="12.75">
@@ -4854,16 +4854,16 @@
         <v>95</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="12.75">
@@ -4871,16 +4871,16 @@
         <v>96</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="12.75">
@@ -4888,16 +4888,16 @@
         <v>97</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="12.75">
@@ -4905,16 +4905,16 @@
         <v>98</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="12.75">
@@ -4922,16 +4922,16 @@
         <v>99</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="12.75">
@@ -4939,16 +4939,16 @@
         <v>100</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="12.75">
@@ -4956,16 +4956,16 @@
         <v>101</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="12.75">
@@ -4973,16 +4973,16 @@
         <v>102</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="12.75">
@@ -4990,16 +4990,16 @@
         <v>103</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="12.75">
@@ -5007,16 +5007,16 @@
         <v>104</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="12.75">
@@ -5024,16 +5024,16 @@
         <v>105</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="12.75">
@@ -5041,16 +5041,16 @@
         <v>106</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="12.75">
@@ -5058,16 +5058,16 @@
         <v>107</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="12.75">
@@ -5075,16 +5075,16 @@
         <v>108</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="12.75">
@@ -5092,16 +5092,16 @@
         <v>109</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="12.75">
@@ -5109,16 +5109,16 @@
         <v>110</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="12.75">
@@ -5126,16 +5126,16 @@
         <v>111</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="12.75">
@@ -5143,16 +5143,16 @@
         <v>112</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="12.75">
@@ -5160,16 +5160,16 @@
         <v>113</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="12.75">
@@ -5177,16 +5177,16 @@
         <v>114</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="12.75">
@@ -5194,16 +5194,16 @@
         <v>115</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="12.75">
@@ -5211,16 +5211,16 @@
         <v>116</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="12.75">
@@ -5228,16 +5228,16 @@
         <v>117</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="12.75">
@@ -5245,16 +5245,16 @@
         <v>118</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="12.75">
@@ -5262,16 +5262,16 @@
         <v>119</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="12.75">
@@ -5279,16 +5279,16 @@
         <v>120</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="12.75">
@@ -5296,16 +5296,16 @@
         <v>121</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="12.75">
@@ -5313,16 +5313,16 @@
         <v>122</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="12.75">
@@ -5330,16 +5330,16 @@
         <v>123</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="12.75">
@@ -5347,16 +5347,16 @@
         <v>124</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="12.75">
@@ -5364,16 +5364,16 @@
         <v>125</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="12.75">
@@ -5381,16 +5381,16 @@
         <v>126</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="12.75">
@@ -5398,16 +5398,16 @@
         <v>127</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="12.75">
@@ -5415,16 +5415,16 @@
         <v>128</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="12.75">
@@ -5432,16 +5432,16 @@
         <v>129</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="12.75">
@@ -5449,16 +5449,16 @@
         <v>130</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="12.75">
@@ -5466,16 +5466,16 @@
         <v>131</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="12.75">
@@ -5483,16 +5483,16 @@
         <v>132</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="12.75">
@@ -5500,16 +5500,16 @@
         <v>133</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="12.75">
@@ -5517,16 +5517,16 @@
         <v>134</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="12.75">
@@ -5534,16 +5534,16 @@
         <v>135</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="12.75">
@@ -5551,16 +5551,16 @@
         <v>136</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="12.75">
@@ -5568,16 +5568,16 @@
         <v>137</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="12.75">
@@ -5585,16 +5585,16 @@
         <v>138</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="12.75">
@@ -5602,16 +5602,16 @@
         <v>139</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="12.75">
@@ -5619,16 +5619,16 @@
         <v>140</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="12.75">
@@ -5636,16 +5636,16 @@
         <v>141</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="12.75">
@@ -5653,16 +5653,16 @@
         <v>142</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="12.75">
@@ -5670,16 +5670,16 @@
         <v>143</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="12.75">
@@ -5687,16 +5687,16 @@
         <v>144</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="12.75">
@@ -5704,16 +5704,16 @@
         <v>145</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="12.75">
@@ -5721,16 +5721,16 @@
         <v>146</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="12.75">
@@ -5738,16 +5738,16 @@
         <v>147</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="12.75">
@@ -5755,16 +5755,16 @@
         <v>148</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="12.75">
@@ -5772,16 +5772,16 @@
         <v>149</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="12.75">
@@ -5789,16 +5789,16 @@
         <v>150</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="12.75">
@@ -5806,16 +5806,16 @@
         <v>151</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="12.75">
@@ -5823,16 +5823,16 @@
         <v>152</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="12.75">
@@ -5840,16 +5840,16 @@
         <v>153</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="12.75">
@@ -5857,16 +5857,16 @@
         <v>154</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="12.75">
@@ -5874,16 +5874,16 @@
         <v>155</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="12.75">
@@ -5891,16 +5891,16 @@
         <v>156</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="12.75">
@@ -5908,16 +5908,16 @@
         <v>157</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="12.75">
@@ -5925,16 +5925,16 @@
         <v>158</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="12.75">
@@ -5942,16 +5942,16 @@
         <v>159</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="12.75">
@@ -5959,16 +5959,16 @@
         <v>160</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="12.75">
@@ -5976,16 +5976,16 @@
         <v>161</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="12.75">
@@ -5993,16 +5993,16 @@
         <v>162</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="12.75">
@@ -6010,16 +6010,16 @@
         <v>163</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="12.75">
@@ -6027,16 +6027,16 @@
         <v>164</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="12.75">
@@ -6044,16 +6044,16 @@
         <v>165</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="12.75">
@@ -6061,16 +6061,16 @@
         <v>166</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="12.75">
@@ -6078,16 +6078,16 @@
         <v>167</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="12.75">
@@ -6095,16 +6095,16 @@
         <v>168</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="12.75">
@@ -6112,7 +6112,7 @@
         <v>169</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>629</v>
@@ -6200,13 +6200,13 @@
         <v>648</v>
       </c>
       <c r="C174" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="D174" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="D174" s="2" t="s">
+      <c r="E174" s="2" t="s">
         <v>650</v>
-      </c>
-      <c r="E174" s="2" t="s">
-        <v>651</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="12.75">
@@ -6214,16 +6214,16 @@
         <v>175</v>
       </c>
       <c r="B175" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="C175" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="D175" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="D175" s="2" t="s">
+      <c r="E175" s="2" t="s">
         <v>654</v>
-      </c>
-      <c r="E175" s="2" t="s">
-        <v>655</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="12.75">
@@ -6231,16 +6231,16 @@
         <v>176</v>
       </c>
       <c r="B176" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="C176" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="D176" s="2" t="s">
         <v>657</v>
       </c>
-      <c r="D176" s="2" t="s">
+      <c r="E176" s="2" t="s">
         <v>658</v>
-      </c>
-      <c r="E176" s="2" t="s">
-        <v>659</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="12.75">
@@ -6248,16 +6248,16 @@
         <v>177</v>
       </c>
       <c r="B177" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="C177" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="D177" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D177" s="2" t="s">
+      <c r="E177" s="2" t="s">
         <v>662</v>
-      </c>
-      <c r="E177" s="2" t="s">
-        <v>663</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="12.75">
@@ -6265,16 +6265,16 @@
         <v>178</v>
       </c>
       <c r="B178" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C178" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="C178" s="2" t="s">
+      <c r="D178" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="D178" s="2" t="s">
+      <c r="E178" s="2" t="s">
         <v>666</v>
-      </c>
-      <c r="E178" s="2" t="s">
-        <v>667</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="12.75">
@@ -6282,16 +6282,16 @@
         <v>179</v>
       </c>
       <c r="B179" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="D179" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="C179" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="D179" s="2" t="s">
+      <c r="E179" s="2" t="s">
         <v>669</v>
-      </c>
-      <c r="E179" s="2" t="s">
-        <v>670</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="12.75">
@@ -6299,16 +6299,16 @@
         <v>180</v>
       </c>
       <c r="B180" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="C180" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="C180" s="2" t="s">
+      <c r="D180" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D180" s="2" t="s">
+      <c r="E180" s="2" t="s">
         <v>673</v>
-      </c>
-      <c r="E180" s="2" t="s">
-        <v>674</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="12.75">
@@ -6316,16 +6316,16 @@
         <v>181</v>
       </c>
       <c r="B181" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="D181" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="C181" s="2" t="s">
-        <v>675</v>
-      </c>
-      <c r="D181" s="2" t="s">
+      <c r="E181" s="2" t="s">
         <v>676</v>
-      </c>
-      <c r="E181" s="2" t="s">
-        <v>677</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="12.75">
@@ -6333,16 +6333,16 @@
         <v>182</v>
       </c>
       <c r="B182" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="D182" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="C182" s="2" t="s">
-        <v>678</v>
-      </c>
-      <c r="D182" s="2" t="s">
+      <c r="E182" s="2" t="s">
         <v>679</v>
-      </c>
-      <c r="E182" s="2" t="s">
-        <v>680</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="12.75">
@@ -6350,16 +6350,16 @@
         <v>183</v>
       </c>
       <c r="B183" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="C183" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="C183" s="2" t="s">
+      <c r="D183" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="D183" s="2" t="s">
+      <c r="E183" s="2" t="s">
         <v>683</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>684</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="12.75">
@@ -6367,16 +6367,16 @@
         <v>184</v>
       </c>
       <c r="B184" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="C184" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="D184" s="2" t="s">
         <v>686</v>
       </c>
-      <c r="D184" s="2" t="s">
+      <c r="E184" s="2" t="s">
         <v>687</v>
-      </c>
-      <c r="E184" s="2" t="s">
-        <v>688</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="12.75">
@@ -6384,16 +6384,16 @@
         <v>185</v>
       </c>
       <c r="B185" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="D185" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="C185" s="2" t="s">
-        <v>689</v>
-      </c>
-      <c r="D185" s="2" t="s">
+      <c r="E185" s="2" t="s">
         <v>690</v>
-      </c>
-      <c r="E185" s="2" t="s">
-        <v>691</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="12.75">
@@ -6401,16 +6401,16 @@
         <v>186</v>
       </c>
       <c r="B186" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="C186" s="2" t="s">
         <v>692</v>
       </c>
-      <c r="C186" s="2" t="s">
+      <c r="D186" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="D186" s="2" t="s">
+      <c r="E186" s="2" t="s">
         <v>694</v>
-      </c>
-      <c r="E186" s="2" t="s">
-        <v>695</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="12.75">
@@ -6418,16 +6418,16 @@
         <v>187</v>
       </c>
       <c r="B187" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="D187" s="2" t="s">
         <v>696</v>
       </c>
-      <c r="C187" s="2" t="s">
-        <v>696</v>
-      </c>
-      <c r="D187" s="2" t="s">
+      <c r="E187" s="2" t="s">
         <v>697</v>
-      </c>
-      <c r="E187" s="2" t="s">
-        <v>698</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="12.75">
@@ -6435,16 +6435,16 @@
         <v>188</v>
       </c>
       <c r="B188" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="C188" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="C188" s="2" t="s">
+      <c r="D188" s="2" t="s">
         <v>700</v>
       </c>
-      <c r="D188" s="2" t="s">
+      <c r="E188" s="2" t="s">
         <v>701</v>
-      </c>
-      <c r="E188" s="2" t="s">
-        <v>702</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="12.75">
@@ -6452,16 +6452,16 @@
         <v>189</v>
       </c>
       <c r="B189" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="C189" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="C189" s="2" t="s">
+      <c r="D189" s="2" t="s">
         <v>704</v>
       </c>
-      <c r="D189" s="2" t="s">
+      <c r="E189" s="2" t="s">
         <v>705</v>
-      </c>
-      <c r="E189" s="2" t="s">
-        <v>706</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="12.75">
@@ -6469,16 +6469,16 @@
         <v>190</v>
       </c>
       <c r="B190" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="C190" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="D190" s="2" t="s">
         <v>708</v>
       </c>
-      <c r="D190" s="2" t="s">
+      <c r="E190" s="2" t="s">
         <v>709</v>
-      </c>
-      <c r="E190" s="2" t="s">
-        <v>710</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="12.75">
@@ -6486,16 +6486,16 @@
         <v>191</v>
       </c>
       <c r="B191" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="C191" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="C191" s="2" t="s">
+      <c r="D191" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="D191" s="2" t="s">
+      <c r="E191" s="2" t="s">
         <v>713</v>
-      </c>
-      <c r="E191" s="2" t="s">
-        <v>714</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="12.75">
@@ -6503,16 +6503,16 @@
         <v>192</v>
       </c>
       <c r="B192" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="C192" s="2" t="s">
         <v>715</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="D192" s="2" t="s">
         <v>716</v>
       </c>
-      <c r="D192" s="2" t="s">
+      <c r="E192" s="2" t="s">
         <v>717</v>
-      </c>
-      <c r="E192" s="2" t="s">
-        <v>718</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="12.75">
@@ -6520,16 +6520,16 @@
         <v>193</v>
       </c>
       <c r="B193" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="C193" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="D193" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="D193" s="2" t="s">
+      <c r="E193" s="2" t="s">
         <v>721</v>
-      </c>
-      <c r="E193" s="2" t="s">
-        <v>722</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="12.75">
@@ -6537,16 +6537,16 @@
         <v>194</v>
       </c>
       <c r="B194" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="C194" s="2" t="s">
         <v>723</v>
       </c>
-      <c r="C194" s="2" t="s">
+      <c r="D194" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="D194" s="2" t="s">
+      <c r="E194" s="2" t="s">
         <v>725</v>
-      </c>
-      <c r="E194" s="2" t="s">
-        <v>726</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="12.75">
@@ -6554,16 +6554,16 @@
         <v>195</v>
       </c>
       <c r="B195" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="C195" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="C195" s="2" t="s">
+      <c r="D195" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="D195" s="2" t="s">
+      <c r="E195" s="2" t="s">
         <v>729</v>
-      </c>
-      <c r="E195" s="2" t="s">
-        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="12.75">
@@ -6571,16 +6571,16 @@
         <v>196</v>
       </c>
       <c r="B196" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="D196" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="C196" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="D196" s="2" t="s">
+      <c r="E196" s="2" t="s">
         <v>732</v>
-      </c>
-      <c r="E196" s="2" t="s">
-        <v>733</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="12.75">
@@ -6588,16 +6588,16 @@
         <v>197</v>
       </c>
       <c r="B197" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="D197" s="2" t="s">
         <v>734</v>
       </c>
-      <c r="C197" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="D197" s="2" t="s">
+      <c r="E197" s="2" t="s">
         <v>735</v>
-      </c>
-      <c r="E197" s="2" t="s">
-        <v>736</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="12.75">
@@ -6605,16 +6605,16 @@
         <v>198</v>
       </c>
       <c r="B198" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C198" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="C198" s="2" t="s">
+      <c r="D198" s="2" t="s">
         <v>738</v>
       </c>
-      <c r="D198" s="2" t="s">
+      <c r="E198" s="2" t="s">
         <v>739</v>
-      </c>
-      <c r="E198" s="2" t="s">
-        <v>740</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="12.75">
@@ -6622,16 +6622,16 @@
         <v>199</v>
       </c>
       <c r="B199" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="D199" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="C199" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="D199" s="2" t="s">
+      <c r="E199" s="2" t="s">
         <v>742</v>
-      </c>
-      <c r="E199" s="2" t="s">
-        <v>743</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="12.75">
@@ -6639,16 +6639,16 @@
         <v>200</v>
       </c>
       <c r="B200" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="C200" s="2" t="s">
         <v>744</v>
       </c>
-      <c r="C200" s="2" t="s">
+      <c r="D200" s="2" t="s">
         <v>745</v>
       </c>
-      <c r="D200" s="2" t="s">
+      <c r="E200" s="2" t="s">
         <v>746</v>
-      </c>
-      <c r="E200" s="2" t="s">
-        <v>747</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="12.75">
@@ -6656,16 +6656,16 @@
         <v>201</v>
       </c>
       <c r="B201" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="C201" s="2" t="s">
         <v>748</v>
       </c>
-      <c r="C201" s="2" t="s">
+      <c r="D201" s="2" t="s">
         <v>749</v>
       </c>
-      <c r="D201" s="2" t="s">
+      <c r="E201" s="2" t="s">
         <v>750</v>
-      </c>
-      <c r="E201" s="2" t="s">
-        <v>751</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="12.75">
@@ -6673,16 +6673,16 @@
         <v>202</v>
       </c>
       <c r="B202" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="C202" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="C202" s="2" t="s">
+      <c r="D202" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="D202" s="2" t="s">
+      <c r="E202" s="2" t="s">
         <v>754</v>
-      </c>
-      <c r="E202" s="2" t="s">
-        <v>755</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="12.75">
@@ -6690,16 +6690,16 @@
         <v>203</v>
       </c>
       <c r="B203" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="C203" s="2" t="s">
         <v>756</v>
       </c>
-      <c r="C203" s="2" t="s">
+      <c r="D203" s="2" t="s">
         <v>757</v>
       </c>
-      <c r="D203" s="2" t="s">
+      <c r="E203" s="2" t="s">
         <v>758</v>
-      </c>
-      <c r="E203" s="2" t="s">
-        <v>759</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="12.75">
@@ -6707,16 +6707,16 @@
         <v>204</v>
       </c>
       <c r="B204" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="C204" s="2" t="s">
         <v>760</v>
       </c>
-      <c r="C204" s="2" t="s">
+      <c r="D204" s="2" t="s">
         <v>761</v>
       </c>
-      <c r="D204" s="2" t="s">
+      <c r="E204" s="2" t="s">
         <v>762</v>
-      </c>
-      <c r="E204" s="2" t="s">
-        <v>763</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="12.75">
@@ -6724,16 +6724,16 @@
         <v>205</v>
       </c>
       <c r="B205" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="C205" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="C205" s="2" t="s">
+      <c r="D205" s="2" t="s">
         <v>765</v>
       </c>
-      <c r="D205" s="2" t="s">
+      <c r="E205" s="2" t="s">
         <v>766</v>
-      </c>
-      <c r="E205" s="2" t="s">
-        <v>767</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="12.75">
@@ -6741,16 +6741,16 @@
         <v>206</v>
       </c>
       <c r="B206" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="C206" s="2" t="s">
         <v>768</v>
       </c>
-      <c r="C206" s="2" t="s">
+      <c r="D206" s="2" t="s">
         <v>769</v>
       </c>
-      <c r="D206" s="2" t="s">
+      <c r="E206" s="2" t="s">
         <v>770</v>
-      </c>
-      <c r="E206" s="2" t="s">
-        <v>771</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="12.75">
@@ -6758,16 +6758,16 @@
         <v>207</v>
       </c>
       <c r="B207" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="C207" s="2" t="s">
         <v>772</v>
       </c>
-      <c r="C207" s="2" t="s">
+      <c r="D207" s="2" t="s">
         <v>773</v>
       </c>
-      <c r="D207" s="2" t="s">
+      <c r="E207" s="2" t="s">
         <v>774</v>
-      </c>
-      <c r="E207" s="2" t="s">
-        <v>775</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="12.75">
@@ -6775,16 +6775,16 @@
         <v>208</v>
       </c>
       <c r="B208" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="C208" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="C208" s="2" t="s">
+      <c r="D208" s="2" t="s">
         <v>777</v>
       </c>
-      <c r="D208" s="2" t="s">
+      <c r="E208" s="2" t="s">
         <v>778</v>
-      </c>
-      <c r="E208" s="2" t="s">
-        <v>779</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="12.75">
@@ -6792,16 +6792,16 @@
         <v>209</v>
       </c>
       <c r="B209" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C209" s="2" t="s">
         <v>780</v>
       </c>
-      <c r="C209" s="2" t="s">
+      <c r="D209" s="2" t="s">
         <v>781</v>
       </c>
-      <c r="D209" s="2" t="s">
+      <c r="E209" s="2" t="s">
         <v>782</v>
-      </c>
-      <c r="E209" s="2" t="s">
-        <v>783</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="12.75">
@@ -6809,16 +6809,16 @@
         <v>210</v>
       </c>
       <c r="B210" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="D210" s="2" t="s">
         <v>784</v>
       </c>
-      <c r="C210" s="2" t="s">
+      <c r="E210" s="2" t="s">
         <v>785</v>
-      </c>
-      <c r="D210" s="2" t="s">
-        <v>786</v>
-      </c>
-      <c r="E210" s="2" t="s">
-        <v>787</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="12.75">
@@ -6826,16 +6826,16 @@
         <v>211</v>
       </c>
       <c r="B211" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="E211" s="2" t="s">
         <v>788</v>
-      </c>
-      <c r="C211" s="2" t="s">
-        <v>788</v>
-      </c>
-      <c r="D211" s="2" t="s">
-        <v>789</v>
-      </c>
-      <c r="E211" s="2" t="s">
-        <v>790</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="12.75">
@@ -6843,16 +6843,16 @@
         <v>212</v>
       </c>
       <c r="B212" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="E212" s="2" t="s">
         <v>791</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>791</v>
-      </c>
-      <c r="D212" s="2" t="s">
-        <v>792</v>
-      </c>
-      <c r="E212" s="2" t="s">
-        <v>793</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="12.75">
@@ -6860,16 +6860,16 @@
         <v>213</v>
       </c>
       <c r="B213" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="D213" s="2" t="s">
         <v>794</v>
       </c>
-      <c r="C213" s="2" t="s">
+      <c r="E213" s="2" t="s">
         <v>795</v>
-      </c>
-      <c r="D213" s="2" t="s">
-        <v>796</v>
-      </c>
-      <c r="E213" s="2" t="s">
-        <v>797</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="12.75">
@@ -6877,16 +6877,16 @@
         <v>214</v>
       </c>
       <c r="B214" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="D214" s="2" t="s">
         <v>798</v>
       </c>
-      <c r="C214" s="2" t="s">
+      <c r="E214" s="2" t="s">
         <v>799</v>
-      </c>
-      <c r="D214" s="2" t="s">
-        <v>800</v>
-      </c>
-      <c r="E214" s="2" t="s">
-        <v>801</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="12.75">
@@ -6894,16 +6894,16 @@
         <v>215</v>
       </c>
       <c r="B215" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="D215" s="2" t="s">
         <v>802</v>
       </c>
-      <c r="C215" s="2" t="s">
+      <c r="E215" s="2" t="s">
         <v>803</v>
-      </c>
-      <c r="D215" s="2" t="s">
-        <v>804</v>
-      </c>
-      <c r="E215" s="2" t="s">
-        <v>805</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="12.75">
@@ -6911,16 +6911,16 @@
         <v>216</v>
       </c>
       <c r="B216" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="D216" s="2" t="s">
         <v>806</v>
       </c>
-      <c r="C216" s="2" t="s">
+      <c r="E216" s="2" t="s">
         <v>807</v>
-      </c>
-      <c r="D216" s="2" t="s">
-        <v>808</v>
-      </c>
-      <c r="E216" s="2" t="s">
-        <v>809</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="12.75">
@@ -6928,16 +6928,16 @@
         <v>217</v>
       </c>
       <c r="B217" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="D217" s="2" t="s">
         <v>810</v>
       </c>
-      <c r="C217" s="2" t="s">
+      <c r="E217" s="2" t="s">
         <v>811</v>
-      </c>
-      <c r="D217" s="2" t="s">
-        <v>812</v>
-      </c>
-      <c r="E217" s="2" t="s">
-        <v>813</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="218" customHeight="1" ht="12.75">
@@ -6945,16 +6945,16 @@
         <v>218</v>
       </c>
       <c r="B218" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="E218" s="2" t="s">
         <v>814</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>814</v>
-      </c>
-      <c r="D218" s="2" t="s">
-        <v>815</v>
-      </c>
-      <c r="E218" s="2" t="s">
-        <v>816</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="12.75">
@@ -6962,16 +6962,16 @@
         <v>219</v>
       </c>
       <c r="B219" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="E219" s="2" t="s">
         <v>817</v>
-      </c>
-      <c r="C219" s="2" t="s">
-        <v>817</v>
-      </c>
-      <c r="D219" s="2" t="s">
-        <v>818</v>
-      </c>
-      <c r="E219" s="2" t="s">
-        <v>819</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="220" customHeight="1" ht="12.75">
@@ -6979,16 +6979,16 @@
         <v>220</v>
       </c>
       <c r="B220" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="D220" s="2" t="s">
         <v>820</v>
       </c>
-      <c r="C220" s="2" t="s">
+      <c r="E220" s="2" t="s">
         <v>821</v>
-      </c>
-      <c r="D220" s="2" t="s">
-        <v>822</v>
-      </c>
-      <c r="E220" s="2" t="s">
-        <v>823</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="12.75">
@@ -6996,16 +6996,16 @@
         <v>221</v>
       </c>
       <c r="B221" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="D221" s="2" t="s">
         <v>824</v>
       </c>
-      <c r="C221" s="2" t="s">
+      <c r="E221" s="2" t="s">
         <v>825</v>
-      </c>
-      <c r="D221" s="2" t="s">
-        <v>826</v>
-      </c>
-      <c r="E221" s="2" t="s">
-        <v>827</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="12.75">
@@ -7013,16 +7013,16 @@
         <v>222</v>
       </c>
       <c r="B222" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="D222" s="2" t="s">
         <v>828</v>
       </c>
-      <c r="C222" s="2" t="s">
+      <c r="E222" s="2" t="s">
         <v>829</v>
-      </c>
-      <c r="D222" s="2" t="s">
-        <v>830</v>
-      </c>
-      <c r="E222" s="2" t="s">
-        <v>831</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="12.75">
@@ -7030,16 +7030,16 @@
         <v>223</v>
       </c>
       <c r="B223" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="D223" s="2" t="s">
         <v>832</v>
       </c>
-      <c r="C223" s="2" t="s">
+      <c r="E223" s="2" t="s">
         <v>833</v>
-      </c>
-      <c r="D223" s="2" t="s">
-        <v>834</v>
-      </c>
-      <c r="E223" s="2" t="s">
-        <v>835</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="12.75">
@@ -7047,16 +7047,16 @@
         <v>224</v>
       </c>
       <c r="B224" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="D224" s="2" t="s">
         <v>836</v>
       </c>
-      <c r="C224" s="2" t="s">
+      <c r="E224" s="2" t="s">
         <v>837</v>
-      </c>
-      <c r="D224" s="2" t="s">
-        <v>838</v>
-      </c>
-      <c r="E224" s="2" t="s">
-        <v>839</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="12.75">
@@ -7064,16 +7064,16 @@
         <v>225</v>
       </c>
       <c r="B225" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="E225" s="2" t="s">
         <v>840</v>
-      </c>
-      <c r="C225" s="2" t="s">
-        <v>840</v>
-      </c>
-      <c r="D225" s="2" t="s">
-        <v>841</v>
-      </c>
-      <c r="E225" s="2" t="s">
-        <v>842</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="12.75">
@@ -7081,16 +7081,16 @@
         <v>226</v>
       </c>
       <c r="B226" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="D226" s="2" t="s">
         <v>843</v>
       </c>
-      <c r="C226" s="2" t="s">
+      <c r="E226" s="2" t="s">
         <v>844</v>
-      </c>
-      <c r="D226" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="E226" s="2" t="s">
-        <v>846</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="12.75">
@@ -7098,16 +7098,16 @@
         <v>227</v>
       </c>
       <c r="B227" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="D227" s="2" t="s">
         <v>847</v>
       </c>
-      <c r="C227" s="2" t="s">
+      <c r="E227" s="2" t="s">
         <v>848</v>
-      </c>
-      <c r="D227" s="2" t="s">
-        <v>849</v>
-      </c>
-      <c r="E227" s="2" t="s">
-        <v>850</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="12.75">
@@ -7115,16 +7115,16 @@
         <v>228</v>
       </c>
       <c r="B228" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="D228" s="2" t="s">
         <v>851</v>
       </c>
-      <c r="C228" s="2" t="s">
+      <c r="E228" s="2" t="s">
         <v>852</v>
-      </c>
-      <c r="D228" s="2" t="s">
-        <v>853</v>
-      </c>
-      <c r="E228" s="2" t="s">
-        <v>854</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="12.75">
@@ -7132,16 +7132,16 @@
         <v>229</v>
       </c>
       <c r="B229" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="E229" s="2" t="s">
         <v>855</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>855</v>
-      </c>
-      <c r="D229" s="2" t="s">
-        <v>856</v>
-      </c>
-      <c r="E229" s="2" t="s">
-        <v>857</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="12.75">
@@ -7149,16 +7149,16 @@
         <v>230</v>
       </c>
       <c r="B230" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="E230" s="2" t="s">
         <v>858</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>858</v>
-      </c>
-      <c r="D230" s="2" t="s">
-        <v>859</v>
-      </c>
-      <c r="E230" s="2" t="s">
-        <v>860</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="12.75">
@@ -7166,16 +7166,16 @@
         <v>231</v>
       </c>
       <c r="B231" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="D231" s="2" t="s">
         <v>861</v>
       </c>
-      <c r="C231" s="2" t="s">
+      <c r="E231" s="2" t="s">
         <v>862</v>
-      </c>
-      <c r="D231" s="2" t="s">
-        <v>863</v>
-      </c>
-      <c r="E231" s="2" t="s">
-        <v>864</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="12.75">
@@ -7183,16 +7183,16 @@
         <v>232</v>
       </c>
       <c r="B232" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="D232" s="2" t="s">
         <v>865</v>
       </c>
-      <c r="C232" s="2" t="s">
+      <c r="E232" s="2" t="s">
         <v>866</v>
-      </c>
-      <c r="D232" s="2" t="s">
-        <v>867</v>
-      </c>
-      <c r="E232" s="2" t="s">
-        <v>868</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="12.75">
@@ -7200,16 +7200,16 @@
         <v>233</v>
       </c>
       <c r="B233" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="D233" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="C233" s="2" t="s">
+      <c r="E233" s="2" t="s">
         <v>870</v>
-      </c>
-      <c r="D233" s="2" t="s">
-        <v>871</v>
-      </c>
-      <c r="E233" s="2" t="s">
-        <v>872</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="12.75">
@@ -7217,16 +7217,16 @@
         <v>234</v>
       </c>
       <c r="B234" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="D234" s="2" t="s">
         <v>873</v>
       </c>
-      <c r="C234" s="2" t="s">
+      <c r="E234" s="2" t="s">
         <v>874</v>
-      </c>
-      <c r="D234" s="2" t="s">
-        <v>875</v>
-      </c>
-      <c r="E234" s="2" t="s">
-        <v>876</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="12.75">
@@ -7234,16 +7234,16 @@
         <v>235</v>
       </c>
       <c r="B235" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D235" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="E235" s="2" t="s">
         <v>877</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>877</v>
-      </c>
-      <c r="D235" s="2" t="s">
-        <v>878</v>
-      </c>
-      <c r="E235" s="2" t="s">
-        <v>879</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="236" customHeight="1" ht="12.75">
@@ -7251,16 +7251,16 @@
         <v>237</v>
       </c>
       <c r="B236" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="D236" s="2" t="s">
         <v>880</v>
       </c>
-      <c r="C236" s="2" t="s">
+      <c r="E236" s="2" t="s">
         <v>881</v>
-      </c>
-      <c r="D236" s="2" t="s">
-        <v>882</v>
-      </c>
-      <c r="E236" s="2" t="s">
-        <v>883</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="237" customHeight="1" ht="12.75">
@@ -7268,16 +7268,16 @@
         <v>238</v>
       </c>
       <c r="B237" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="D237" s="2" t="s">
         <v>884</v>
       </c>
-      <c r="C237" s="2" t="s">
+      <c r="E237" s="2" t="s">
         <v>885</v>
-      </c>
-      <c r="D237" s="2" t="s">
-        <v>886</v>
-      </c>
-      <c r="E237" s="2" t="s">
-        <v>887</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="238" customHeight="1" ht="12.75">
@@ -7285,16 +7285,16 @@
         <v>239</v>
       </c>
       <c r="B238" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="D238" s="2" t="s">
         <v>888</v>
       </c>
-      <c r="C238" s="2" t="s">
+      <c r="E238" s="2" t="s">
         <v>889</v>
-      </c>
-      <c r="D238" s="2" t="s">
-        <v>890</v>
-      </c>
-      <c r="E238" s="2" t="s">
-        <v>891</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="239" customHeight="1" ht="12.75">
@@ -7302,16 +7302,16 @@
         <v>242</v>
       </c>
       <c r="B239" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="D239" s="2" t="s">
         <v>892</v>
       </c>
-      <c r="C239" s="2" t="s">
+      <c r="E239" s="2" t="s">
         <v>893</v>
-      </c>
-      <c r="D239" s="2" t="s">
-        <v>894</v>
-      </c>
-      <c r="E239" s="2" t="s">
-        <v>895</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="12.75">
@@ -7319,16 +7319,16 @@
         <v>243</v>
       </c>
       <c r="B240" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="D240" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="C240" s="2" t="s">
+      <c r="E240" s="2" t="s">
         <v>897</v>
-      </c>
-      <c r="D240" s="2" t="s">
-        <v>898</v>
-      </c>
-      <c r="E240" s="2" t="s">
-        <v>899</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="241" customHeight="1" ht="12.75">
@@ -7336,16 +7336,16 @@
         <v>244</v>
       </c>
       <c r="B241" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="D241" s="2" t="s">
         <v>900</v>
       </c>
-      <c r="C241" s="2" t="s">
+      <c r="E241" s="2" t="s">
         <v>901</v>
-      </c>
-      <c r="D241" s="2" t="s">
-        <v>902</v>
-      </c>
-      <c r="E241" s="2" t="s">
-        <v>903</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="242" customHeight="1" ht="12.75">
@@ -7353,16 +7353,16 @@
         <v>245</v>
       </c>
       <c r="B242" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="D242" s="2" t="s">
         <v>904</v>
       </c>
-      <c r="C242" s="2" t="s">
+      <c r="E242" s="2" t="s">
         <v>905</v>
-      </c>
-      <c r="D242" s="2" t="s">
-        <v>906</v>
-      </c>
-      <c r="E242" s="2" t="s">
-        <v>907</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="243" customHeight="1" ht="12.75">
@@ -7370,16 +7370,16 @@
         <v>246</v>
       </c>
       <c r="B243" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="D243" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="E243" s="2" t="s">
         <v>908</v>
-      </c>
-      <c r="C243" s="2" t="s">
-        <v>908</v>
-      </c>
-      <c r="D243" s="2" t="s">
-        <v>909</v>
-      </c>
-      <c r="E243" s="2" t="s">
-        <v>910</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="12.75">
@@ -7387,16 +7387,16 @@
         <v>247</v>
       </c>
       <c r="B244" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="D244" s="2" t="s">
         <v>911</v>
       </c>
-      <c r="C244" s="2" t="s">
+      <c r="E244" s="2" t="s">
         <v>912</v>
-      </c>
-      <c r="D244" s="2" t="s">
-        <v>913</v>
-      </c>
-      <c r="E244" s="2" t="s">
-        <v>914</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="245" customHeight="1" ht="12.75">
@@ -7404,16 +7404,16 @@
         <v>248</v>
       </c>
       <c r="B245" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="D245" s="2" t="s">
         <v>915</v>
       </c>
-      <c r="C245" s="2" t="s">
+      <c r="E245" s="2" t="s">
         <v>916</v>
-      </c>
-      <c r="D245" s="2" t="s">
-        <v>917</v>
-      </c>
-      <c r="E245" s="2" t="s">
-        <v>918</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="246" customHeight="1" ht="12.75">
@@ -7421,16 +7421,16 @@
         <v>249</v>
       </c>
       <c r="B246" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="E246" s="2" t="s">
         <v>919</v>
-      </c>
-      <c r="C246" s="2" t="s">
-        <v>919</v>
-      </c>
-      <c r="D246" s="2" t="s">
-        <v>920</v>
-      </c>
-      <c r="E246" s="2" t="s">
-        <v>921</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="12.75">
@@ -7438,16 +7438,16 @@
         <v>250</v>
       </c>
       <c r="B247" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="D247" s="2" t="s">
         <v>922</v>
       </c>
-      <c r="C247" s="2" t="s">
+      <c r="E247" s="2" t="s">
         <v>923</v>
-      </c>
-      <c r="D247" s="2" t="s">
-        <v>924</v>
-      </c>
-      <c r="E247" s="2" t="s">
-        <v>925</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="12.75">
@@ -7455,16 +7455,16 @@
         <v>251</v>
       </c>
       <c r="B248" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="D248" s="2" t="s">
         <v>926</v>
       </c>
-      <c r="C248" s="2" t="s">
+      <c r="E248" s="2" t="s">
         <v>927</v>
-      </c>
-      <c r="D248" s="2" t="s">
-        <v>928</v>
-      </c>
-      <c r="E248" s="2" t="s">
-        <v>929</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="12.75">
@@ -7472,16 +7472,16 @@
         <v>252</v>
       </c>
       <c r="B249" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="D249" s="2" t="s">
         <v>930</v>
       </c>
-      <c r="C249" s="2" t="s">
+      <c r="E249" s="2" t="s">
         <v>931</v>
-      </c>
-      <c r="D249" s="2" t="s">
-        <v>932</v>
-      </c>
-      <c r="E249" s="2" t="s">
-        <v>933</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="12.75">
@@ -7489,16 +7489,16 @@
         <v>253</v>
       </c>
       <c r="B250" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="D250" s="2" t="s">
         <v>934</v>
       </c>
-      <c r="C250" s="2" t="s">
+      <c r="E250" s="2" t="s">
         <v>935</v>
-      </c>
-      <c r="D250" s="2" t="s">
-        <v>936</v>
-      </c>
-      <c r="E250" s="2" t="s">
-        <v>937</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="12.75">
@@ -7506,16 +7506,16 @@
         <v>254</v>
       </c>
       <c r="B251" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="D251" s="2" t="s">
         <v>938</v>
       </c>
-      <c r="C251" s="2" t="s">
+      <c r="E251" s="2" t="s">
         <v>939</v>
-      </c>
-      <c r="D251" s="2" t="s">
-        <v>940</v>
-      </c>
-      <c r="E251" s="2" t="s">
-        <v>941</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="252" customHeight="1" ht="12.75">
@@ -7523,16 +7523,16 @@
         <v>255</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="E252" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="12.75">
@@ -7540,16 +7540,16 @@
         <v>256</v>
       </c>
       <c r="B253" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="E253" s="2" t="s">
         <v>944</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>944</v>
-      </c>
-      <c r="D253" s="2" t="s">
-        <v>945</v>
-      </c>
-      <c r="E253" s="2" t="s">
-        <v>946</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="12.75">
@@ -7557,16 +7557,16 @@
         <v>257</v>
       </c>
       <c r="B254" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="E254" s="2" t="s">
         <v>947</v>
-      </c>
-      <c r="C254" s="2" t="s">
-        <v>947</v>
-      </c>
-      <c r="D254" s="2" t="s">
-        <v>948</v>
-      </c>
-      <c r="E254" s="2" t="s">
-        <v>949</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="255" customHeight="1" ht="12.75">

</xml_diff>